<commit_message>
- BC BanHang: tonghop,chitiet,nhomhang: add column {ThanhTienTruocCK, TienChietKhau}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoBanHang/Teamplate_BaoCaoBanHangChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoBanHang/Teamplate_BaoCaoBanHangChiTiet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>BÁO CÁO BÁN HÀNG CHI TIẾT</t>
   </si>
@@ -116,6 +116,10 @@
   </si>
   <si>
     <t>Chi phí</t>
+  </si>
+  <si>
+    <t>Thành tiền 
+(trước CK)</t>
   </si>
 </sst>
 </file>
@@ -663,11 +667,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF29"/>
+  <dimension ref="A1:AG29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,21 +690,22 @@
     <col min="14" max="14" width="20.7109375" style="26" customWidth="1"/>
     <col min="15" max="15" width="16.42578125" style="29" customWidth="1"/>
     <col min="16" max="16" width="14.7109375" style="29" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" style="29" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="29" customWidth="1"/>
-    <col min="19" max="22" width="14.7109375" style="29" customWidth="1"/>
-    <col min="23" max="23" width="18" style="29" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="18" style="29" customWidth="1"/>
-    <col min="26" max="26" width="21" style="16" customWidth="1"/>
-    <col min="27" max="27" width="19.42578125" style="24" customWidth="1"/>
-    <col min="28" max="28" width="18" style="16" customWidth="1"/>
-    <col min="29" max="29" width="21.28515625" style="7" customWidth="1"/>
-    <col min="30" max="30" width="25.85546875" style="16" customWidth="1"/>
-    <col min="31" max="31" width="25.85546875" style="21" customWidth="1"/>
-    <col min="32" max="16384" width="9.140625" style="1"/>
+    <col min="17" max="17" width="24.85546875" style="29" customWidth="1"/>
+    <col min="18" max="18" width="16.42578125" style="29" customWidth="1"/>
+    <col min="19" max="19" width="18.28515625" style="29" customWidth="1"/>
+    <col min="20" max="23" width="14.7109375" style="29" customWidth="1"/>
+    <col min="24" max="24" width="18" style="29" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="18" style="29" customWidth="1"/>
+    <col min="27" max="27" width="21" style="16" customWidth="1"/>
+    <col min="28" max="28" width="19.42578125" style="24" customWidth="1"/>
+    <col min="29" max="29" width="18" style="16" customWidth="1"/>
+    <col min="30" max="30" width="21.28515625" style="7" customWidth="1"/>
+    <col min="31" max="31" width="25.85546875" style="16" customWidth="1"/>
+    <col min="32" max="32" width="25.85546875" style="21" customWidth="1"/>
+    <col min="33" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
@@ -734,9 +739,10 @@
       <c r="AC1" s="33"/>
       <c r="AD1" s="33"/>
       <c r="AE1" s="33"/>
-      <c r="AF1" s="2"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF1" s="33"/>
+      <c r="AG1" s="2"/>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="34"/>
       <c r="B2" s="34"/>
       <c r="C2" s="34"/>
@@ -768,13 +774,14 @@
       <c r="AC2" s="34"/>
       <c r="AD2" s="34"/>
       <c r="AE2" s="34"/>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AF2" s="34"/>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="17"/>
       <c r="C3" s="17"/>
       <c r="G3" s="17"/>
     </row>
-    <row r="4" spans="1:32" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -824,52 +831,55 @@
         <v>16</v>
       </c>
       <c r="Q4" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="30" t="s">
+      <c r="S4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="30" t="s">
+      <c r="T4" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="30" t="s">
+      <c r="U4" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="30" t="s">
+      <c r="V4" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="V4" s="30" t="s">
+      <c r="W4" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="W4" s="30" t="s">
+      <c r="X4" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="X4" s="30" t="s">
+      <c r="Y4" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="Y4" s="30" t="s">
+      <c r="Z4" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="Z4" s="11" t="s">
+      <c r="AA4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA4" s="9" t="s">
+      <c r="AB4" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AB4" s="11" t="s">
+      <c r="AC4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AC4" s="11" t="s">
+      <c r="AD4" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD4" s="11" t="s">
+      <c r="AE4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AE4" s="11" t="s">
+      <c r="AF4" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="20"/>
       <c r="C5" s="3"/>
@@ -895,14 +905,15 @@
       <c r="W5" s="31"/>
       <c r="X5" s="31"/>
       <c r="Y5" s="31"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="22"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="14"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="22"/>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="20"/>
       <c r="C6" s="3"/>
@@ -928,14 +939,15 @@
       <c r="W6" s="31"/>
       <c r="X6" s="31"/>
       <c r="Y6" s="31"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="25"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="22"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z6" s="31"/>
+      <c r="AA6" s="14"/>
+      <c r="AB6" s="25"/>
+      <c r="AC6" s="14"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="14"/>
+      <c r="AF6" s="22"/>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="20"/>
       <c r="C7" s="3"/>
@@ -961,14 +973,15 @@
       <c r="W7" s="31"/>
       <c r="X7" s="31"/>
       <c r="Y7" s="31"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="25"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="22"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z7" s="31"/>
+      <c r="AA7" s="14"/>
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="14"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="14"/>
+      <c r="AF7" s="22"/>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="20"/>
       <c r="C8" s="3"/>
@@ -994,14 +1007,15 @@
       <c r="W8" s="31"/>
       <c r="X8" s="31"/>
       <c r="Y8" s="31"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="25"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="22"/>
-    </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z8" s="31"/>
+      <c r="AA8" s="14"/>
+      <c r="AB8" s="25"/>
+      <c r="AC8" s="14"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="14"/>
+      <c r="AF8" s="22"/>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="20"/>
       <c r="C9" s="3"/>
@@ -1027,14 +1041,15 @@
       <c r="W9" s="31"/>
       <c r="X9" s="31"/>
       <c r="Y9" s="31"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="25"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="22"/>
-    </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z9" s="31"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="25"/>
+      <c r="AC9" s="14"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="14"/>
+      <c r="AF9" s="22"/>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="20"/>
       <c r="C10" s="3"/>
@@ -1060,14 +1075,15 @@
       <c r="W10" s="31"/>
       <c r="X10" s="31"/>
       <c r="Y10" s="31"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="25"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="22"/>
-    </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="14"/>
+      <c r="AB10" s="25"/>
+      <c r="AC10" s="14"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="14"/>
+      <c r="AF10" s="22"/>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="20"/>
       <c r="C11" s="3"/>
@@ -1093,14 +1109,15 @@
       <c r="W11" s="31"/>
       <c r="X11" s="31"/>
       <c r="Y11" s="31"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="25"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="22"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z11" s="31"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="25"/>
+      <c r="AC11" s="14"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="22"/>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="20"/>
       <c r="C12" s="3"/>
@@ -1126,14 +1143,15 @@
       <c r="W12" s="31"/>
       <c r="X12" s="31"/>
       <c r="Y12" s="31"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="25"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="22"/>
-    </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z12" s="31"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="25"/>
+      <c r="AC12" s="14"/>
+      <c r="AD12" s="6"/>
+      <c r="AE12" s="14"/>
+      <c r="AF12" s="22"/>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="20"/>
       <c r="C13" s="3"/>
@@ -1159,14 +1177,15 @@
       <c r="W13" s="31"/>
       <c r="X13" s="31"/>
       <c r="Y13" s="31"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="25"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="14"/>
-      <c r="AE13" s="22"/>
-    </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z13" s="31"/>
+      <c r="AA13" s="14"/>
+      <c r="AB13" s="25"/>
+      <c r="AC13" s="14"/>
+      <c r="AD13" s="6"/>
+      <c r="AE13" s="14"/>
+      <c r="AF13" s="22"/>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="20"/>
       <c r="C14" s="3"/>
@@ -1192,14 +1211,15 @@
       <c r="W14" s="31"/>
       <c r="X14" s="31"/>
       <c r="Y14" s="31"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="25"/>
-      <c r="AB14" s="14"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="14"/>
-      <c r="AE14" s="22"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="25"/>
+      <c r="AC14" s="14"/>
+      <c r="AD14" s="6"/>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="22"/>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="20"/>
       <c r="C15" s="3"/>
@@ -1225,14 +1245,15 @@
       <c r="W15" s="31"/>
       <c r="X15" s="31"/>
       <c r="Y15" s="31"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="25"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="22"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Z15" s="31"/>
+      <c r="AA15" s="14"/>
+      <c r="AB15" s="25"/>
+      <c r="AC15" s="14"/>
+      <c r="AD15" s="6"/>
+      <c r="AE15" s="14"/>
+      <c r="AF15" s="22"/>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="20"/>
       <c r="C16" s="3"/>
@@ -1258,14 +1279,15 @@
       <c r="W16" s="31"/>
       <c r="X16" s="31"/>
       <c r="Y16" s="31"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="25"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="22"/>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="14"/>
+      <c r="AB16" s="25"/>
+      <c r="AC16" s="14"/>
+      <c r="AD16" s="6"/>
+      <c r="AE16" s="14"/>
+      <c r="AF16" s="22"/>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="20"/>
       <c r="C17" s="3"/>
@@ -1291,14 +1313,15 @@
       <c r="W17" s="31"/>
       <c r="X17" s="31"/>
       <c r="Y17" s="31"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="25"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="22"/>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z17" s="31"/>
+      <c r="AA17" s="14"/>
+      <c r="AB17" s="25"/>
+      <c r="AC17" s="14"/>
+      <c r="AD17" s="6"/>
+      <c r="AE17" s="14"/>
+      <c r="AF17" s="22"/>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="20"/>
       <c r="C18" s="3"/>
@@ -1324,14 +1347,15 @@
       <c r="W18" s="31"/>
       <c r="X18" s="31"/>
       <c r="Y18" s="31"/>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="25"/>
-      <c r="AB18" s="14"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="14"/>
-      <c r="AE18" s="22"/>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="14"/>
+      <c r="AB18" s="25"/>
+      <c r="AC18" s="14"/>
+      <c r="AD18" s="6"/>
+      <c r="AE18" s="14"/>
+      <c r="AF18" s="22"/>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="20"/>
       <c r="C19" s="3"/>
@@ -1357,14 +1381,15 @@
       <c r="W19" s="31"/>
       <c r="X19" s="31"/>
       <c r="Y19" s="31"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="25"/>
-      <c r="AB19" s="14"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="14"/>
-      <c r="AE19" s="22"/>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z19" s="31"/>
+      <c r="AA19" s="14"/>
+      <c r="AB19" s="25"/>
+      <c r="AC19" s="14"/>
+      <c r="AD19" s="6"/>
+      <c r="AE19" s="14"/>
+      <c r="AF19" s="22"/>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="20"/>
       <c r="C20" s="3"/>
@@ -1390,14 +1415,15 @@
       <c r="W20" s="31"/>
       <c r="X20" s="31"/>
       <c r="Y20" s="31"/>
-      <c r="Z20" s="14"/>
-      <c r="AA20" s="25"/>
-      <c r="AB20" s="14"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="14"/>
-      <c r="AE20" s="22"/>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="14"/>
+      <c r="AB20" s="25"/>
+      <c r="AC20" s="14"/>
+      <c r="AD20" s="6"/>
+      <c r="AE20" s="14"/>
+      <c r="AF20" s="22"/>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="20"/>
       <c r="C21" s="3"/>
@@ -1423,14 +1449,15 @@
       <c r="W21" s="31"/>
       <c r="X21" s="31"/>
       <c r="Y21" s="31"/>
-      <c r="Z21" s="14"/>
-      <c r="AA21" s="25"/>
-      <c r="AB21" s="14"/>
-      <c r="AC21" s="6"/>
-      <c r="AD21" s="14"/>
-      <c r="AE21" s="22"/>
-    </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z21" s="31"/>
+      <c r="AA21" s="14"/>
+      <c r="AB21" s="25"/>
+      <c r="AC21" s="14"/>
+      <c r="AD21" s="6"/>
+      <c r="AE21" s="14"/>
+      <c r="AF21" s="22"/>
+    </row>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="20"/>
       <c r="C22" s="3"/>
@@ -1456,14 +1483,15 @@
       <c r="W22" s="31"/>
       <c r="X22" s="31"/>
       <c r="Y22" s="31"/>
-      <c r="Z22" s="14"/>
-      <c r="AA22" s="25"/>
-      <c r="AB22" s="14"/>
-      <c r="AC22" s="6"/>
-      <c r="AD22" s="14"/>
-      <c r="AE22" s="22"/>
-    </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="14"/>
+      <c r="AB22" s="25"/>
+      <c r="AC22" s="14"/>
+      <c r="AD22" s="6"/>
+      <c r="AE22" s="14"/>
+      <c r="AF22" s="22"/>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="20"/>
       <c r="C23" s="3"/>
@@ -1489,14 +1517,15 @@
       <c r="W23" s="31"/>
       <c r="X23" s="31"/>
       <c r="Y23" s="31"/>
-      <c r="Z23" s="14"/>
-      <c r="AA23" s="25"/>
-      <c r="AB23" s="14"/>
-      <c r="AC23" s="6"/>
-      <c r="AD23" s="14"/>
-      <c r="AE23" s="22"/>
-    </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z23" s="31"/>
+      <c r="AA23" s="14"/>
+      <c r="AB23" s="25"/>
+      <c r="AC23" s="14"/>
+      <c r="AD23" s="6"/>
+      <c r="AE23" s="14"/>
+      <c r="AF23" s="22"/>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" s="20"/>
       <c r="C24" s="3"/>
@@ -1522,14 +1551,15 @@
       <c r="W24" s="31"/>
       <c r="X24" s="31"/>
       <c r="Y24" s="31"/>
-      <c r="Z24" s="14"/>
-      <c r="AA24" s="25"/>
-      <c r="AB24" s="14"/>
-      <c r="AC24" s="6"/>
-      <c r="AD24" s="14"/>
-      <c r="AE24" s="22"/>
-    </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z24" s="31"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="25"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="6"/>
+      <c r="AE24" s="14"/>
+      <c r="AF24" s="22"/>
+    </row>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="20"/>
       <c r="C25" s="3"/>
@@ -1555,14 +1585,15 @@
       <c r="W25" s="31"/>
       <c r="X25" s="31"/>
       <c r="Y25" s="31"/>
-      <c r="Z25" s="14"/>
-      <c r="AA25" s="25"/>
-      <c r="AB25" s="14"/>
-      <c r="AC25" s="6"/>
-      <c r="AD25" s="14"/>
-      <c r="AE25" s="22"/>
-    </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="14"/>
+      <c r="AB25" s="25"/>
+      <c r="AC25" s="14"/>
+      <c r="AD25" s="6"/>
+      <c r="AE25" s="14"/>
+      <c r="AF25" s="22"/>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="20"/>
       <c r="C26" s="3"/>
@@ -1588,14 +1619,15 @@
       <c r="W26" s="31"/>
       <c r="X26" s="31"/>
       <c r="Y26" s="31"/>
-      <c r="Z26" s="14"/>
-      <c r="AA26" s="25"/>
-      <c r="AB26" s="14"/>
-      <c r="AC26" s="6"/>
-      <c r="AD26" s="14"/>
-      <c r="AE26" s="22"/>
-    </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z26" s="31"/>
+      <c r="AA26" s="14"/>
+      <c r="AB26" s="25"/>
+      <c r="AC26" s="14"/>
+      <c r="AD26" s="6"/>
+      <c r="AE26" s="14"/>
+      <c r="AF26" s="22"/>
+    </row>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" s="20"/>
       <c r="C27" s="3"/>
@@ -1621,14 +1653,15 @@
       <c r="W27" s="31"/>
       <c r="X27" s="31"/>
       <c r="Y27" s="31"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="25"/>
-      <c r="AB27" s="14"/>
-      <c r="AC27" s="6"/>
-      <c r="AD27" s="14"/>
-      <c r="AE27" s="22"/>
-    </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="Z27" s="31"/>
+      <c r="AA27" s="14"/>
+      <c r="AB27" s="25"/>
+      <c r="AC27" s="14"/>
+      <c r="AD27" s="6"/>
+      <c r="AE27" s="14"/>
+      <c r="AF27" s="22"/>
+    </row>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="20"/>
       <c r="C28" s="3"/>
@@ -1654,14 +1687,15 @@
       <c r="W28" s="31"/>
       <c r="X28" s="31"/>
       <c r="Y28" s="31"/>
-      <c r="Z28" s="14"/>
-      <c r="AA28" s="25"/>
-      <c r="AB28" s="14"/>
-      <c r="AC28" s="6"/>
-      <c r="AD28" s="14"/>
-      <c r="AE28" s="22"/>
-    </row>
-    <row r="29" spans="1:31" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Z28" s="31"/>
+      <c r="AA28" s="14"/>
+      <c r="AB28" s="25"/>
+      <c r="AC28" s="14"/>
+      <c r="AD28" s="6"/>
+      <c r="AE28" s="14"/>
+      <c r="AF28" s="22"/>
+    </row>
+    <row r="29" spans="1:32" s="8" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="35" t="s">
         <v>1</v>
       </c>
@@ -1683,7 +1717,10 @@
         <v>0</v>
       </c>
       <c r="P29" s="32"/>
-      <c r="Q29" s="32"/>
+      <c r="Q29" s="32">
+        <f>SUM(Q$5:Q28)</f>
+        <v>0</v>
+      </c>
       <c r="R29" s="32">
         <f>SUM(R$5:R28)</f>
         <v>0</v>
@@ -1700,11 +1737,11 @@
         <f>SUM(U$5:U28)</f>
         <v>0</v>
       </c>
-      <c r="V29" s="32"/>
-      <c r="W29" s="32">
-        <f>SUM(W$5:W28)</f>
+      <c r="V29" s="32">
+        <f>SUM(V$5:V28)</f>
         <v>0</v>
       </c>
+      <c r="W29" s="32"/>
       <c r="X29" s="32">
         <f>SUM(X$5:X28)</f>
         <v>0</v>
@@ -1713,17 +1750,21 @@
         <f>SUM(Y$5:Y28)</f>
         <v>0</v>
       </c>
-      <c r="Z29" s="15"/>
+      <c r="Z29" s="32">
+        <f>SUM(Z$5:Z28)</f>
+        <v>0</v>
+      </c>
       <c r="AA29" s="15"/>
       <c r="AB29" s="15"/>
-      <c r="AC29" s="13"/>
-      <c r="AD29" s="15"/>
-      <c r="AE29" s="23"/>
+      <c r="AC29" s="15"/>
+      <c r="AD29" s="13"/>
+      <c r="AE29" s="15"/>
+      <c r="AF29" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:AE1"/>
-    <mergeCell ref="A2:AE2"/>
+    <mergeCell ref="A1:AF1"/>
+    <mergeCell ref="A2:AF2"/>
     <mergeCell ref="A29:N29"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>

</xml_diff>